<commit_message>
fixed prompt for cot stats
</commit_message>
<xml_diff>
--- a/experiment_data/cot_data/cot_data_input.xlsx
+++ b/experiment_data/cot_data/cot_data_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\OneDrive\Desktop\Codenames Progetto PDE\Codenames-LLM\experiment_data\cot_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frmar\OneDrive\Desktop\GitHub\Codenames-LLM\experiment_data\cot_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582D2256-D996-40C2-8C55-0C21D612C42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6244047-2EEF-4063-90F8-6710582D9B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="2952" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="14">
   <si>
     <t>winner</t>
   </si>
@@ -424,23 +424,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -691,194 +694,194 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -894,6 +897,390 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>13</v>
+      </c>
+      <c r="B84" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>13</v>
+      </c>
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>13</v>
+      </c>
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>13</v>
+      </c>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>13</v>
+      </c>
+      <c r="B92" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>13</v>
+      </c>
+      <c r="B93" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>13</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>13</v>
+      </c>
+      <c r="B95" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>13</v>
+      </c>
+      <c r="B96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>13</v>
+      </c>
+      <c r="B97" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>13</v>
+      </c>
+      <c r="B98" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>13</v>
+      </c>
+      <c r="B99" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>13</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>13</v>
+      </c>
+      <c r="B101" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>